<commit_message>
Added enums + drivers + a lot of refactoring
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Data.xlsx
+++ b/src/main/resources/excel/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="LogConfigs" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="LoginConfigs" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="DriverConfigs" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="BusinessConfigs" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -90,10 +90,10 @@
     <t>src/main/resources/chromedriver.exe</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>src/main/resources/MicrosoftWebDriver.exe</t>
+    <t>src/main/resources/geckodriver.exe</t>
+  </si>
+  <si>
+    <t>src/main/resources/msedgedriver.exe</t>
   </si>
   <si>
     <t>BASE_URL</t>
@@ -479,7 +479,7 @@
     <col customWidth="1" min="2" max="2" width="21.86"/>
     <col customWidth="1" min="3" max="3" width="19.86"/>
     <col customWidth="1" min="4" max="4" width="34.29"/>
-    <col customWidth="1" min="5" max="5" width="28.71"/>
+    <col customWidth="1" min="5" max="5" width="32.0"/>
     <col customWidth="1" min="6" max="6" width="39.57"/>
     <col customWidth="1" min="7" max="7" width="30.29"/>
   </cols>
@@ -520,10 +520,10 @@
       <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="1">

</xml_diff>

<commit_message>
Added properties file, exceptions, +some refactoring
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/Data.xlsx
+++ b/src/main/resources/excel/Data.xlsx
@@ -4,8 +4,6 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="LoginConfigs" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="DriverConfigs" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="BusinessConfigs" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Email</t>
   </si>
@@ -36,6 +34,9 @@
     <t>64CHAR_EMAIL</t>
   </si>
   <si>
+    <t>INCORRECT_PASSWORD</t>
+  </si>
+  <si>
     <t>ivanhorintest@gmail.com</t>
   </si>
   <si>
@@ -57,68 +58,14 @@
     <t>exampleexampleexampleexampleexampleexampleexampleexampleexamplee@gmail.com</t>
   </si>
   <si>
-    <t>CHROME_NAME</t>
-  </si>
-  <si>
-    <t>FIREFOX_NAME</t>
-  </si>
-  <si>
-    <t>EDGE_NAME</t>
-  </si>
-  <si>
-    <t>CHROME_DRIVER_LOCATION</t>
-  </si>
-  <si>
-    <t>FIREFOX_DRIVER_LOCATION</t>
-  </si>
-  <si>
-    <t>EDGE_DRIVER_LOCATION</t>
-  </si>
-  <si>
-    <t>IMPLICITLY_WAIT_VALUE</t>
-  </si>
-  <si>
-    <t>webdriver.chrome.driver</t>
-  </si>
-  <si>
-    <t>webdriver.gecko.driver</t>
-  </si>
-  <si>
-    <t>webdriver.edge.driver</t>
-  </si>
-  <si>
-    <t>src/main/resources/chromedriver.exe</t>
-  </si>
-  <si>
-    <t>src/main/resources/geckodriver.exe</t>
-  </si>
-  <si>
-    <t>src/main/resources/msedgedriver.exe</t>
-  </si>
-  <si>
-    <t>BASE_URL</t>
-  </si>
-  <si>
-    <t>HOME_PAGE_URL</t>
-  </si>
-  <si>
-    <t>TRAINING_LIST_PAGE_URL</t>
-  </si>
-  <si>
-    <t>https://training.by</t>
-  </si>
-  <si>
-    <t>/#/Home</t>
-  </si>
-  <si>
-    <t>/#!/TrainingList</t>
+    <t>incorrectPassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -132,14 +79,9 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -162,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -172,13 +114,7 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -190,14 +126,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -412,6 +340,7 @@
     <col customWidth="1" min="5" max="5" width="18.43"/>
     <col customWidth="1" min="6" max="6" width="81.0"/>
     <col customWidth="1" min="7" max="7" width="77.71"/>
+    <col customWidth="1" min="8" max="8" width="29.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -427,7 +356,7 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -435,147 +364,38 @@
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="2" width="21.86"/>
-    <col customWidth="1" min="3" max="3" width="19.86"/>
-    <col customWidth="1" min="4" max="4" width="34.29"/>
-    <col customWidth="1" min="5" max="5" width="32.0"/>
-    <col customWidth="1" min="6" max="6" width="39.57"/>
-    <col customWidth="1" min="7" max="7" width="30.29"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="16.29"/>
-    <col customWidth="1" min="2" max="2" width="18.57"/>
-    <col customWidth="1" min="3" max="3" width="26.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>